<commit_message>
Build v2.1.5: Hotfix: Omit empty descriptions for parameters and schemas
</commit_message>
<xml_diff>
--- a/tests/legacy_converter/fixtures/R1_basic_structure/expected/$index.xlsx
+++ b/tests/legacy_converter/fixtures/R1_basic_structure/expected/$index.xlsx
@@ -721,7 +721,7 @@
       </c>
       <c r="B2" s="24" t="inlineStr">
         <is>
-          <t>This is a test API for legacy converter validation.</t>
+          <t>A test API</t>
         </is>
       </c>
       <c r="C2" s="25" t="n"/>
@@ -783,7 +783,7 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>/int/test</t>
+          <t>servers description</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -791,11 +791,7 @@
           <t>servers description</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>Integration Test</t>
-        </is>
-      </c>
+      <c r="D7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -805,7 +801,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>/test</t>
+          <t>servers description</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
@@ -813,11 +809,7 @@
           <t>servers description</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>Production</t>
-        </is>
-      </c>
+      <c r="D8" s="3" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -938,44 +930,38 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>/test/{testId}</t>
+          <t>/test</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>testOperation</t>
+          <t>post</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>post</t>
+          <t>Test Op</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>A test operation for validation</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>TestTag</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Test operation summary</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>testOperation</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>x-custom-field: custom-value
-x-another: value2</t>
-        </is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v/>
+      </c>
+      <c r="G3" t="n">
+        <v/>
+      </c>
+      <c r="H3" t="n">
+        <v/>
+      </c>
+      <c r="I3" t="n">
+        <v/>
+      </c>
+      <c r="J3" t="n">
+        <v/>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="22"/>
@@ -1051,18 +1037,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TestTag</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>TestTag</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
     <row r="3"/>
     <row r="4"/>
     <row r="5"/>
@@ -1086,7 +1061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1187,38 +1162,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>testId</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>The unique test identifier</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>path</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="list">
@@ -1236,7 +1179,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1329,33 +1272,6 @@
       <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Example</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>X-Correlation-Id</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Request correlation identifier</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>50</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1401,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>searchCriteria</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1495,12 +1411,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Search criteria container</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>TestId</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -1512,497 +1433,62 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dateFrom</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>searchCriteria</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Start date</t>
+          <t>testOperationResponse</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>TestDate</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>M</t>
+          <t>object</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>dateTo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>searchCriteria</t>
+          <t>TestId</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>End date</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>TestDate</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>O</t>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>int64</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>testName</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>testOperationRequest</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>The test name</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>TestName</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>amount</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>testOperationRequest</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>The amount</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>TestAmount</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>testOperationRequest</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>The status</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>TestStatus</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>testOperationResponse</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>resultData</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>testOperationResponse</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Result container</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>result</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>resultData</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>The processed result</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>TestName</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>processedDate</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>resultData</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Date of processing</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>TestDate</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>testOperationResponse</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Response status</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>schema</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>TestStatus</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>TestName</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>A test name field</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>140</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>^[A-Za-z]+$</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>ExampleTestName</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>TestAmount</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>A monetary amount</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>double</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>999999.99</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>1234.56</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>TestStatus</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Status indicator</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>ACTIVE; INACTIVE; PENDING</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>ACTIVE</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>TestDate</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>A date field</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>2026-02-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>TestId</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Unique identifier</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>abc-123-def</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>CorrelationId</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Request correlation identifier</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>corr-12345</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Generic object container</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-    </row>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
     <row r="21"/>
     <row r="22"/>
     <row r="23"/>
@@ -3573,7 +3059,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3680,18 +3166,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>

</xml_diff>